<commit_message>
Finished HW1 UG and Prog
</commit_message>
<xml_diff>
--- a/HW1/janka.xlsx
+++ b/HW1/janka.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24501"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F11E5BF1-2469-4BD8-81D0-3C12792CF247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1494A558-EE64-4CF1-8AFA-216A33073683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -98,27 +98,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -438,412 +426,413 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3" ht="30">
-      <c r="A1" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>24.7</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>484</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>24.8</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>427</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>27.3</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>413</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>28.4</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>517</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>28.4</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>549</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>29</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>648</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>30.3</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>587</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>32.700000000000003</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>704</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>35.6</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>979</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>38.5</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>514</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>38.799999999999997</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>1070</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>39.299999999999997</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>1020</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>39.4</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>1210</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>39.9</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>989</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>40.299999999999997</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>1160</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>40.36</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>1010</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>40.700000000000003</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>1100</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>40.700000000000003</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>1130</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>42.9</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>1270</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="3">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>45.8</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>1180</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="3">
+      <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>46.9</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>1400</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="3">
+      <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>48.2</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>1760</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="3">
+      <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>51.5</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>1710</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="3">
+      <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>51.5</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>2010</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="3">
+      <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>53.4</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>1880</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="3">
+      <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>56</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>1980</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="3">
+      <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>56.5</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="2">
         <v>1820</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="3">
+      <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>57.3</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="2">
         <v>2020</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="3">
+      <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>57.6</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="2">
         <v>1980</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="3">
+      <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <v>59.2</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="2">
         <v>2310</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="3">
+      <c r="A32" s="2">
         <v>31</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>59.8</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="2">
         <v>1940</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="3">
+      <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>66</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="2">
         <v>3260</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="3">
+      <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <v>37.4</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="2">
         <v>2700</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="3">
+      <c r="A35" s="2">
         <v>34</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="2">
         <v>68.8</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="2">
         <v>2890</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="3">
+      <c r="A36" s="2">
         <v>35</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="2">
         <v>69.099999999999994</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="2">
         <v>2740</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="3">
+      <c r="A37" s="2">
         <v>36</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="2">
         <v>69.099999999999994</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="2">
         <v>3140</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed excel file" '
</commit_message>
<xml_diff>
--- a/HW1/janka.xlsx
+++ b/HW1/janka.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24501"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB2B6398-913D-49A0-A686-71ECC6DD0B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7584F561-FBAD-4FD2-8B50-E41C769EC07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,19 +38,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -77,10 +71,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,413 +391,412 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>24.7</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>484</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>24.8</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>427</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>27.3</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>413</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>28.4</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>517</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>28.4</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>549</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>29</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>648</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>30.3</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>587</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>32.700000000000003</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>704</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>35.6</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>979</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>38.5</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>914</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>38.799999999999997</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>1070</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>39.299999999999997</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>1020</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>39.4</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>1210</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>39.9</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>989</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>40.299999999999997</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>1160</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>40.6</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>1010</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>40.700000000000003</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>1100</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>40.700000000000003</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>1130</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>42.9</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>1270</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>45.8</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>1180</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>46.9</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>1400</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>48.2</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>1760</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>51.5</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>1710</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>51.5</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>2010</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>53.4</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <v>1880</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="2">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>56</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <v>1980</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>56.5</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <v>1820</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="2">
+      <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>57.3</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <v>2020</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>57.6</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <v>1980</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="2">
+      <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>59.2</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <v>2310</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="2">
+      <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>59.8</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <v>1940</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="2">
+      <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>66</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="1">
         <v>3260</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>67.400000000000006</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="1">
         <v>2700</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="2">
+      <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>68.8</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="1">
         <v>2890</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="2">
+      <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>69.099999999999994</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="1">
         <v>2740</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="2">
+      <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="1">
         <v>69.099999999999994</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="1">
         <v>3140</v>
       </c>
     </row>

</xml_diff>